<commit_message>
Postęp backendu i refactor Reacta
</commit_message>
<xml_diff>
--- a/Tracks.xlsx
+++ b/Tracks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\C#\SpotifyApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C402D0-6713-4C56-BFF4-F6A421C2E152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142EDB64-6253-485B-9C79-9DDA4E42F3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CF3BE979-8F5C-41E1-B99A-A9C51CF51F90}"/>
+    <workbookView xWindow="13170" yWindow="1845" windowWidth="26265" windowHeight="14550" xr2:uid="{CF3BE979-8F5C-41E1-B99A-A9C51CF51F90}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Tracks</t>
   </si>
@@ -157,6 +157,36 @@
   </si>
   <si>
     <t>TrackNumber</t>
+  </si>
+  <si>
+    <t>Playlists</t>
+  </si>
+  <si>
+    <t>Items [List&lt;SimplePlaylist&gt;]</t>
+  </si>
+  <si>
+    <t>Collaborative</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ExternalURLs</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>FullTrack -&gt; Artist[0] -&gt; Id -&gt; List&lt;ArtistsRequest&gt;[IList&lt;string&gt; [50]]-&gt;List&lt;ArtistsResponse&gt; -&gt; List&lt;FullArtist&gt; -&gt; Genre</t>
+  </si>
+  <si>
+    <t>Tracks [c]</t>
   </si>
 </sst>
 </file>
@@ -173,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +222,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -205,10 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -523,16 +567,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA1C676-14E0-4648-B217-18CB3794D036}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:O90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -857,24 +901,131 @@
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C78" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>